<commit_message>
Fixed some date bugs
Made date even more strict with input, now accepts only MM/DD/YYYY
Final Test Plan Uploaded
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve_000\Documents\GitHub\trackTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Input</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Task</t>
   </si>
   <si>
-    <t>"Pooh Bear"</t>
-  </si>
-  <si>
     <t>Shows Racer Result</t>
   </si>
   <si>
@@ -56,18 +53,12 @@
     <t>Search by ID (Hash Table Search)</t>
   </si>
   <si>
-    <t>K0098983</t>
-  </si>
-  <si>
     <t>Add a Racer</t>
   </si>
   <si>
     <t xml:space="preserve">Name: Barack Obama </t>
   </si>
   <si>
-    <t>ID: A1234567</t>
-  </si>
-  <si>
     <t>Circuit: White House</t>
   </si>
   <si>
@@ -104,40 +95,91 @@
     <t>I</t>
   </si>
   <si>
-    <t>Remove by License</t>
-  </si>
-  <si>
-    <t>D 000 000 2</t>
-  </si>
-  <si>
-    <t>Undo</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
-    <t>Display Hash and BST to show its gone</t>
-  </si>
-  <si>
-    <t>D, P</t>
-  </si>
-  <si>
-    <t>Display Hash and BST to show its back</t>
-  </si>
-  <si>
     <t>Save hash table output to file</t>
   </si>
   <si>
     <t>O</t>
   </si>
   <si>
-    <t>Saves hash table to be reimported</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>Enter in filename</t>
+  </si>
+  <si>
+    <t>inputRacer.txt</t>
+  </si>
+  <si>
+    <t>Display Items</t>
+  </si>
+  <si>
+    <t>P or D</t>
+  </si>
+  <si>
+    <t>P is Tree, D is hash</t>
+  </si>
+  <si>
+    <t>S + "Pooh Bear"</t>
+  </si>
+  <si>
+    <t>F + "K0098983"</t>
+  </si>
+  <si>
+    <t>ID: A1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Barack Obama </t>
+  </si>
+  <si>
+    <t>R + "A1234"</t>
+  </si>
+  <si>
+    <t>Removes Barack</t>
+  </si>
+  <si>
+    <t>Display and Print to Show Gone</t>
+  </si>
+  <si>
+    <t>D + P</t>
+  </si>
+  <si>
+    <t>Undo delete</t>
+  </si>
+  <si>
+    <t>barack back</t>
+  </si>
+  <si>
+    <t>Display and Print to show its back</t>
+  </si>
+  <si>
+    <t>Show undo Z again</t>
+  </si>
+  <si>
+    <t>"No previous commands"</t>
+  </si>
+  <si>
+    <t>Barack is gone again!</t>
+  </si>
+  <si>
+    <t>Z again</t>
+  </si>
+  <si>
+    <t>Add Someone</t>
+  </si>
+  <si>
+    <t>George Bush</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>A000</t>
+  </si>
+  <si>
+    <t>Date: 01/21/13 Laptime: 100</t>
   </si>
 </sst>
 </file>
@@ -464,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,154 +532,219 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>